<commit_message>
lab5: task 5 is done, task 6 is started
</commit_message>
<xml_diff>
--- a/lab5/данные для лабы 5.xlsx
+++ b/lab5/данные для лабы 5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rfkfi\Desktop\Stepan Orlov\programming university\RGU\lab5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2598CC-AD9F-432A-B165-A84E3945F910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD66333-9F17-4E7D-A609-303B1E9AE5DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="task 3" sheetId="1" r:id="rId1"/>
@@ -662,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -712,8 +712,8 @@
         <v>45635.151800462962</v>
       </c>
       <c r="K1" t="str">
-        <f>SUBSTITUTE(A1," ","_")&amp;" "&amp;SUBSTITUTE(B1," ","_")&amp;" "&amp;C1&amp;" "&amp;D1&amp;" "&amp;E1&amp;" "&amp;F1&amp;" "&amp;SUBSTITUTE(TEXT(G1,"0,00"),",",".")&amp;" "&amp;H1&amp;" "&amp;SUBSTITUTE(TEXT(I1,"ДД:ММ:ГГГГ_ЧЧ:ММ:СС")," ","_")&amp;" "&amp;SUBSTITUTE(TEXT(J1,"ДД:ММ:ГГГГ_ЧЧ:ММ:СС")," ","_")</f>
-        <v>Tokyo Baker_Street 63 T 35 497354 88.50 79630055021329 27:11:2024_10:50:36 09:12:2024_3:38:36</v>
+        <f>SUBSTITUTE(A1," ","_")&amp;" "&amp;SUBSTITUTE(B1," ","_")&amp;" "&amp;C1&amp;" "&amp;D1&amp;" "&amp;E1&amp;" "&amp;F1&amp;" "&amp;SUBSTITUTE(TEXT(G1,"0,00"),",",".")&amp;" "&amp;H1&amp;" "&amp;SUBSTITUTE(TEXT(I1,"ДД:ММ:ГГГГ_ЧЧ:ММ:СС")," "," ")&amp;" "&amp;SUBSTITUTE(TEXT(J1,"ДД:ММ:ГГГГ_ЧЧ:ММ:СС")," "," ")</f>
+        <v>Tokyo Baker_Street 63 T 35 497354 88.50 79630055021329 27:11:2024 10:50:36 09:12:2024 3:38:36</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -749,8 +749,8 @@
         <v>45624.451800462964</v>
       </c>
       <c r="K2" t="str">
-        <f t="shared" ref="K2:K20" si="1">SUBSTITUTE(A2," ","_")&amp;" "&amp;SUBSTITUTE(B2," ","_")&amp;" "&amp;C2&amp;" "&amp;D2&amp;" "&amp;E2&amp;" "&amp;F2&amp;" "&amp;SUBSTITUTE(TEXT(G2,"0,00"),",",".")&amp;" "&amp;H2&amp;" "&amp;SUBSTITUTE(TEXT(I2,"ДД:ММ:ГГГГ_ЧЧ:ММ:СС")," ","_")&amp;" "&amp;SUBSTITUTE(TEXT(J2,"ДД:ММ:ГГГГ_ЧЧ:ММ:СС")," ","_")</f>
-        <v>Paris Champs-Élysées 96 P 157 514556 0.32 59910348646652 27:11:2024_10:50:36 28:11:2024_10:50:36</v>
+        <f t="shared" ref="K2:K20" si="1">SUBSTITUTE(A2," ","_")&amp;" "&amp;SUBSTITUTE(B2," ","_")&amp;" "&amp;C2&amp;" "&amp;D2&amp;" "&amp;E2&amp;" "&amp;F2&amp;" "&amp;SUBSTITUTE(TEXT(G2,"0,00"),",",".")&amp;" "&amp;H2&amp;" "&amp;SUBSTITUTE(TEXT(I2,"ДД:ММ:ГГГГ_ЧЧ:ММ:СС")," "," ")&amp;" "&amp;SUBSTITUTE(TEXT(J2,"ДД:ММ:ГГГГ_ЧЧ:ММ:СС")," "," ")</f>
+        <v>Paris Champs-Élysées 96 P 157 514556 0.32 59910348646652 27:11:2024 10:50:36 28:11:2024 10:50:36</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -787,7 +787,7 @@
       </c>
       <c r="K3" t="str">
         <f t="shared" si="1"/>
-        <v>Sydney Orchard_Road 31 S 123 167834 1.54 59681960757936 27:11:2024_10:50:36 04:12:2024_10:50:36</v>
+        <v>Sydney Orchard_Road 31 S 123 167834 1.54 59681960757936 27:11:2024 10:50:36 04:12:2024 10:50:36</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -824,7 +824,7 @@
       </c>
       <c r="K4" t="str">
         <f t="shared" si="1"/>
-        <v>Cairo Wall_Street 35 C 139 862013 10.67 74678650187110 27:11:2024_10:50:36 06:12:2024_10:50:36</v>
+        <v>Cairo Wall_Street 35 C 139 862013 10.67 74678650187110 27:11:2024 10:50:36 06:12:2024 10:50:36</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -861,7 +861,7 @@
       </c>
       <c r="K5" t="str">
         <f t="shared" si="1"/>
-        <v>Rio_de_Janeiro Nevsky_Prospekt 74 R 96 320666 1.81 71491089520895 27:11:2024_10:50:36 04:12:2024_10:50:36</v>
+        <v>Rio_de_Janeiro Nevsky_Prospekt 74 R 96 320666 1.81 71491089520895 27:11:2024 10:50:36 04:12:2024 10:50:36</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -898,7 +898,7 @@
       </c>
       <c r="K6" t="str">
         <f t="shared" si="1"/>
-        <v>Istanbul Abbey_Road 54 I 43 830775 5.88 27944065585649 27:11:2024_10:50:36 07:12:2024_10:50:36</v>
+        <v>Istanbul Abbey_Road 54 I 43 830775 5.88 27944065585649 27:11:2024 10:50:36 07:12:2024 10:50:36</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -935,7 +935,7 @@
       </c>
       <c r="K7" t="str">
         <f t="shared" si="1"/>
-        <v>Cape_Town Rodeo_Drive 85 C 198 564915 13.83 56932984608628 27:11:2024_10:50:36 03:12:2024_10:50:36</v>
+        <v>Cape_Town Rodeo_Drive 85 C 198 564915 13.83 56932984608628 27:11:2024 10:50:36 03:12:2024 10:50:36</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -972,7 +972,7 @@
       </c>
       <c r="K8" t="str">
         <f t="shared" si="1"/>
-        <v>Toronto Via_del_Corso 35 T 81 383272 4.82 83450203338344 27:11:2024_10:50:36 30:11:2024_10:50:36</v>
+        <v>Toronto Via_del_Corso 35 T 81 383272 4.82 83450203338344 27:11:2024 10:50:36 30:11:2024 10:50:36</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -1009,7 +1009,7 @@
       </c>
       <c r="K9" t="str">
         <f t="shared" si="1"/>
-        <v>Moscow Avenida_Paulista 58 M 105 882865 12.71 74690304012435 27:11:2024_10:50:36 06:12:2024_10:50:36</v>
+        <v>Moscow Avenida_Paulista 58 M 105 882865 12.71 74690304012435 27:11:2024 10:50:36 06:12:2024 10:50:36</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -1046,7 +1046,7 @@
       </c>
       <c r="K10" t="str">
         <f t="shared" si="1"/>
-        <v>Buenos_Aires Arbat_Street 70 B 40 542716 1.29 67872404180867 27:11:2024_10:50:36 28:11:2024_10:50:36</v>
+        <v>Buenos_Aires Arbat_Street 70 B 40 542716 1.29 67872404180867 27:11:2024 10:50:36 28:11:2024 10:50:36</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -1083,7 +1083,7 @@
       </c>
       <c r="K11" t="str">
         <f t="shared" si="1"/>
-        <v>Bangkok Sunset_Boulevard 89 B 147 681922 15.08 17755350253582 27:11:2024_10:50:36 03:12:2024_10:50:36</v>
+        <v>Bangkok Sunset_Boulevard 89 B 147 681922 15.08 17755350253582 27:11:2024 10:50:36 03:12:2024 10:50:36</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -1120,7 +1120,7 @@
       </c>
       <c r="K12" t="str">
         <f t="shared" si="1"/>
-        <v>Berlin Friedrichstraße 85 B 128 987614 14.26 95533174862946 27:11:2024_10:50:36 28:11:2024_10:50:36</v>
+        <v>Berlin Friedrichstraße 85 B 128 987614 14.26 95533174862946 27:11:2024 10:50:36 28:11:2024 10:50:36</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1157,7 +1157,7 @@
       </c>
       <c r="K13" t="str">
         <f t="shared" si="1"/>
-        <v>Nairobi Nathan_Road 11 N 13 612332 45.00 25820214042258 27:11:2024_10:50:36 28:11:2024_10:50:36</v>
+        <v>Nairobi Nathan_Road 11 N 13 612332 45.00 25820214042258 27:11:2024 10:50:36 28:11:2024 10:50:36</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -1194,7 +1194,7 @@
       </c>
       <c r="K14" t="str">
         <f t="shared" si="1"/>
-        <v>Lima Ginza_Street 14 L 180 818799 3.91 64896258324149 27:11:2024_10:50:36 07:12:2024_10:50:36</v>
+        <v>Lima Ginza_Street 14 L 180 818799 3.91 64896258324149 27:11:2024 10:50:36 07:12:2024 10:50:36</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -1231,7 +1231,7 @@
       </c>
       <c r="K15" t="str">
         <f t="shared" si="1"/>
-        <v>Seoul Kurfürstendamm 46 S 54 649745 7.18 19673776053458 27:11:2024_10:50:36 05:12:2024_10:50:36</v>
+        <v>Seoul Kurfürstendamm 46 S 54 649745 7.18 19673776053458 27:11:2024 10:50:36 05:12:2024 10:50:36</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -1268,7 +1268,7 @@
       </c>
       <c r="K16" t="str">
         <f t="shared" si="1"/>
-        <v>Dubai Las_Ramblas 17 D 44 444449 89.64 69712812660894 27:11:2024_10:50:36 28:11:2024_10:50:36</v>
+        <v>Dubai Las_Ramblas 17 D 44 444449 89.64 69712812660894 27:11:2024 10:50:36 28:11:2024 10:50:36</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -1305,7 +1305,7 @@
       </c>
       <c r="K17" t="str">
         <f t="shared" si="1"/>
-        <v>New_York_City Michigan_Avenue 80 N 142 458615 25.21 41762744333471 27:11:2024_10:50:36 30:11:2024_10:50:36</v>
+        <v>New_York_City Michigan_Avenue 80 N 142 458615 25.21 41762744333471 27:11:2024 10:50:36 30:11:2024 10:50:36</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -1342,7 +1342,7 @@
       </c>
       <c r="K18" t="str">
         <f t="shared" si="1"/>
-        <v>Reykjavik Collins_Street 10 R 26 264709 1.29 44891458258470 27:11:2024_10:50:36 03:12:2024_10:50:36</v>
+        <v>Reykjavik Collins_Street 10 R 26 264709 1.29 44891458258470 27:11:2024 10:50:36 03:12:2024 10:50:36</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -1379,7 +1379,7 @@
       </c>
       <c r="K19" t="str">
         <f t="shared" si="1"/>
-        <v>Mumbai Gran_Vía 57 M 114 479525 8.38 42241823929173 27:11:2024_10:50:36 03:12:2024_10:50:36</v>
+        <v>Mumbai Gran_Vía 57 M 114 479525 8.38 42241823929173 27:11:2024 10:50:36 03:12:2024 10:50:36</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -1416,7 +1416,7 @@
       </c>
       <c r="K20" t="str">
         <f t="shared" si="1"/>
-        <v>Athens Istiklal_Avenue 59 A 165 418275 1.65 93232871959794 27:11:2024_10:50:36 02:12:2024_10:50:36</v>
+        <v>Athens Istiklal_Avenue 59 A 165 418275 1.65 93232871959794 27:11:2024 10:50:36 02:12:2024 10:50:36</v>
       </c>
     </row>
   </sheetData>
@@ -1773,8 +1773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D825BA71-546D-4A8C-B323-2025E51E8CC0}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>